<commit_message>
[200~changes for themes and cultural context vocabularies
</commit_message>
<xml_diff>
--- a/installationdocs/02.1_PlacesMapping.xlsx
+++ b/installationdocs/02.1_PlacesMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/o_ugur_exeter_ac_uk/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ou213\OneDrive - University of Exeter\Desktop\git\metadata-schema\installationdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60A3E881-B09C-4720-9014-DB656851FF31}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E5517E-A133-47EB-9C1F-81E93F4F54B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="1185" windowWidth="13425" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Rule type</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>ca_places.preferred_labels</t>
+  </si>
+  <si>
+    <t>ca_places.access</t>
   </si>
 </sst>
 </file>
@@ -340,10 +343,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -612,16 +611,16 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
     <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -664,7 +663,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -677,7 +676,7 @@
       <c r="D3" s="6"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -689,25 +688,31 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="8"/>
+    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="2"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="2"/>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
@@ -723,7 +728,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -742,7 +747,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -761,7 +766,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -780,7 +785,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -798,7 +803,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -813,7 +818,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -829,7 +834,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -845,7 +850,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -861,7 +866,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -882,7 +887,7 @@
       <c r="H17" s="11"/>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>16</v>
       </c>

</xml_diff>